<commit_message>
code etc updated to match the paper
</commit_message>
<xml_diff>
--- a/code/data/numbers/lcdm-free.xlsx
+++ b/code/data/numbers/lcdm-free.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/852b2bada49559ee/code_final/data/numbers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_085D38BF95627E0F6235547658AC46F99AE18372" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{063D2D47-3685-4E29-A3EE-FE1B80A03110}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_085D38BF95627E0F6235547658AC46F99AE18372" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B31E2E8-D05D-4C44-BFEE-38124897D290}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="18720" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -463,11 +463,12 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="31.61328125" customWidth="1"/>
     <col min="2" max="3" width="9.23046875" style="3"/>
     <col min="4" max="4" width="9.23046875" style="6"/>
     <col min="5" max="6" width="9.23046875" style="3"/>

</xml_diff>